<commit_message>
Interação básica com o editor
Um pouco de JS para controlar a interface
</commit_message>
<xml_diff>
--- a/editor.xlsx
+++ b/editor.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Nome</t>
   </si>
@@ -122,15 +122,9 @@
     <t>Define como o objeto deve estar alinhado na página (-1 = esquerda, 0 = centralizado, 1 = direita)</t>
   </si>
   <si>
-    <t>\{[:alinhamento:] [:string:] 0\}</t>
-  </si>
-  <si>
     <t>\{[:alinhamento:] [:string:] 1\}</t>
   </si>
   <si>
-    <t>\{[:alinhamento:] [:imagem:] 2\}</t>
-  </si>
-  <si>
     <t>Objeto de régua</t>
   </si>
   <si>
@@ -182,12 +176,6 @@
     <t>\{([:subIndice:]|[:folhaIndice:]( [:subIndice:]| [:folhaIndice:])*)?\}</t>
   </si>
   <si>
-    <t>\{[1-9] [:string:] [:string:] [:indice:] [:paginas:] [:anexos:] [:strings:]\}</t>
-  </si>
-  <si>
-    <t>Um livro é o texto todo, com os dados e meta-dados: a versão do formato (atual = 1), o nome, as opções de edição (formato definido pelo editor), o índice, as páginas, os anexos e o conteúdo string de cada página</t>
-  </si>
-  <si>
     <t>Strings</t>
   </si>
   <si>
@@ -198,6 +186,30 @@
   </si>
   <si>
     <t>"[^"]*"</t>
+  </si>
+  <si>
+    <t>\{[1-9] [:string:] [:edicao:] [:indice:] [:paginas:] [:anexos:] [:strings:]\}</t>
+  </si>
+  <si>
+    <t>Opções de edição</t>
+  </si>
+  <si>
+    <t>Um livro é o texto todo, com os dados e meta-dados: a versão do formato (atual = 1), o nome, as opções de edição, o índice, as páginas, os anexos e o conteúdo string de cada página</t>
+  </si>
+  <si>
+    <t>Dados lidos somente pelo editor: data de criação, data de modificação, auto paginação, auto indexação</t>
+  </si>
+  <si>
+    <t>\{[0-9]+ [0-9]+ [01] [01]\}</t>
+  </si>
+  <si>
+    <t>\{[:alinhamento:]( [:string:])* 0\}</t>
+  </si>
+  <si>
+    <t>Representa um objeto de texto simples (cada string é colocada numa linha)</t>
+  </si>
+  <si>
+    <t>\{[:imagem:] 2\}</t>
   </si>
 </sst>
 </file>
@@ -664,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M138"/>
+  <dimension ref="A1:M140"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:E3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -745,16 +757,16 @@
       <c r="A8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -769,16 +781,16 @@
       <c r="K10" s="8"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="C11" s="5" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -796,13 +808,13 @@
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="C13" s="5" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -820,13 +832,13 @@
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="C15" s="5" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -844,13 +856,13 @@
     <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="C17" s="5" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -865,16 +877,16 @@
       <c r="K18" s="8"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="C19" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -889,16 +901,16 @@
       <c r="K20" s="8"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="C21" s="5" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -913,16 +925,16 @@
       <c r="K22" s="8"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="C23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -937,16 +949,16 @@
       <c r="K24" s="8"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="C25" s="5" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -961,16 +973,16 @@
       <c r="K26" s="8"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="C27" s="5" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="G27" s="1"/>
     </row>
@@ -985,16 +997,16 @@
       <c r="K28" s="8"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="C29" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -1009,16 +1021,16 @@
       <c r="K30" s="8"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="C31" s="5" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -1033,16 +1045,16 @@
       <c r="K32" s="8"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="C33" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -1057,16 +1069,16 @@
       <c r="K34" s="8"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="C35" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G35" s="1"/>
     </row>
@@ -1081,16 +1093,16 @@
       <c r="K36" s="8"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="C37" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G37" s="1"/>
     </row>
@@ -1108,13 +1120,13 @@
     <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="C39" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -1129,16 +1141,16 @@
       <c r="K40" s="8"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="C41" s="5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>29</v>
+        <v>37</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="G41" s="1"/>
     </row>
@@ -1153,16 +1165,16 @@
       <c r="K42" s="8"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="C43" s="5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>60</v>
+        <v>34</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="G43" s="1"/>
     </row>
@@ -1180,46 +1192,68 @@
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="C45" s="5" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="F46" s="7"/>
       <c r="G46" s="1"/>
+      <c r="H46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="M46" s="1"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+      <c r="C47" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="49" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="50" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="51" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="52" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="53" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="54" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="55" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="56" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="57" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="58" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="59" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="60" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="61" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="62" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="63" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="64" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="65" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="66" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="67" hidden="1" x14ac:dyDescent="0.25"/>
@@ -1235,8 +1269,8 @@
     <row r="77" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="78" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="79" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="81" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="84" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1294,6 +1328,8 @@
     <row r="136" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="137" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="138" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C3:E3"/>

</xml_diff>

<commit_message>
Texto agora tem uma lista de strings. fixes #3
</commit_message>
<xml_diff>
--- a/editor.xlsx
+++ b/editor.xlsx
@@ -179,9 +179,6 @@
     <t>Strings</t>
   </si>
   <si>
-    <t>Guarda a representação string de cada página, usada para fazer buscas</t>
-  </si>
-  <si>
     <t>\{([:string:]( [:string:])*)?\}</t>
   </si>
   <si>
@@ -203,13 +200,16 @@
     <t>\{[0-9]+ [0-9]+ [01] [01]\}</t>
   </si>
   <si>
-    <t>\{[:alinhamento:]( [:string:])* 0\}</t>
-  </si>
-  <si>
     <t>Representa um objeto de texto simples (cada string é colocada numa linha)</t>
   </si>
   <si>
     <t>\{[:imagem:] 2\}</t>
+  </si>
+  <si>
+    <t>\{[:alinhamento:] [:strings:] 0\}</t>
+  </si>
+  <si>
+    <t>Guarda a representação string de cada página (usada para fazer buscas) ou o texto de cada linha</t>
   </si>
 </sst>
 </file>
@@ -678,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M140"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -763,10 +763,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -784,13 +784,13 @@
     <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="C11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -973,16 +973,16 @@
       <c r="K26" s="8"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="C27" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="G27" s="1"/>
     </row>
@@ -1051,10 +1051,10 @@
         <v>17</v>
       </c>
       <c r="D33" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -1102,7 +1102,7 @@
         <v>24</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G37" s="1"/>
     </row>
@@ -1198,7 +1198,7 @@
         <v>27</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G45" s="1"/>
     </row>

</xml_diff>

<commit_message>
Funções de abrir e salvar livros
</commit_message>
<xml_diff>
--- a/editor.xlsx
+++ b/editor.xlsx
@@ -161,9 +161,6 @@
     <t>\{[:alinhamento:] [:nivel:] [:string:] 3\}</t>
   </si>
   <si>
-    <t>\{[:cor:] [:altura:] 4\}</t>
-  </si>
-  <si>
     <t>Sub índice</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>Guarda a representação string de cada página (usada para fazer buscas) ou o texto de cada linha</t>
+  </si>
+  <si>
+    <t>\{[:altura:] 4\}</t>
   </si>
 </sst>
 </file>
@@ -678,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M140"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -763,10 +763,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -784,13 +784,13 @@
     <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="C11" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -814,7 +814,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -832,13 +832,13 @@
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="C15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -976,13 +976,13 @@
     <row r="27" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="C27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="G27" s="1"/>
     </row>
@@ -1051,10 +1051,10 @@
         <v>17</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -1102,7 +1102,7 @@
         <v>24</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G37" s="1"/>
     </row>
@@ -1150,7 +1150,7 @@
         <v>37</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="G41" s="1"/>
     </row>
@@ -1198,7 +1198,7 @@
         <v>27</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G45" s="1"/>
     </row>

</xml_diff>